<commit_message>
added template sheet in results template
</commit_message>
<xml_diff>
--- a/TDMS_CSI_ExcelTemplates/Result_Collection_Template.xlsx
+++ b/TDMS_CSI_ExcelTemplates/Result_Collection_Template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ENTWICKLUNG\Software\data_automator\TDMS_CSI_ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E8B569-2C4E-445C-8B5D-9877CA082C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A583A50E-5DCF-43CE-9F3D-9684829260F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6756" yWindow="2484" windowWidth="14832" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
+    <sheet name="Charts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -339,14 +340,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T16:15:39, Uncontrolled copy when printed</oddFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:36:51, Uncontrolled copy when printed</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B062105E-B73B-455B-ACB6-ED25B9971D91}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:36:51, Uncontrolled copy when printed</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added basic evaluation on the results template
</commit_message>
<xml_diff>
--- a/TDMS_CSI_ExcelTemplates/Result_Collection_Template.xlsx
+++ b/TDMS_CSI_ExcelTemplates/Result_Collection_Template.xlsx
@@ -8,21 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ENTWICKLUNG\Software\data_automator\TDMS_CSI_ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A583A50E-5DCF-43CE-9F3D-9684829260F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E1011B-B47B-4FFB-82EE-2FD79095D629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2856" windowWidth="14832" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
     <sheet name="Charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Delta Max-Min</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,30 +365,404 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:36:51, Uncontrolled copy when printed</oddFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:45:09, Uncontrolled copy when printed</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B062105E-B73B-455B-ACB6-ED25B9971D91}">
-  <dimension ref="A1"/>
+  <dimension ref="B5:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f>Result!C6</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>MAX(Result!D6:AG6)</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>MIN(Result!D6:AG6)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>C6-D6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f>Result!C7</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>MAX(Result!D7:AG7)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>MIN(Result!D7:AG7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E24" si="0">C7-D7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f>Result!C8</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>MAX(Result!D8:AG8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>MIN(Result!D8:AG8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>Result!C9</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f>MAX(Result!D9:AG9)</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>MIN(Result!D9:AG9)</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <f>Result!C10</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>MAX(Result!D10:AG10)</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>MIN(Result!D10:AG10)</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f>Result!C11</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>MAX(Result!D11:AG11)</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>MIN(Result!D11:AG11)</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>Result!C12</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>MAX(Result!D12:AG12)</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>MIN(Result!D12:AG12)</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>Result!C13</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>MAX(Result!D13:AG13)</f>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>MIN(Result!D13:AG13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <f>Result!C14</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>MAX(Result!D14:AG14)</f>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f>MIN(Result!D14:AG14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>Result!C15</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>MAX(Result!D15:AG15)</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>MIN(Result!D15:AG15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <f>Result!C16</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>MAX(Result!D16:AG16)</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>MIN(Result!D16:AG16)</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f>Result!C17</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>MAX(Result!D17:AG17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>MIN(Result!D17:AG17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f>Result!C18</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>MAX(Result!D18:AG18)</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>MIN(Result!D18:AG18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f>Result!C19</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>MAX(Result!D19:AG19)</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>MIN(Result!D19:AG19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>Result!C20</f>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f>MAX(Result!D20:AG20)</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>MIN(Result!D20:AG20)</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f>Result!C21</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f>MAX(Result!D21:AG21)</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>MIN(Result!D21:AG21)</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>Result!C22</f>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>MAX(Result!D22:AG22)</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>MIN(Result!D22:AG22)</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>Result!C23</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>MAX(Result!D23:AG23)</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>MIN(Result!D23:AG23)</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f>Result!C24</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>MAX(Result!D24:AG24)</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>MIN(Result!D24:AG24)</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E6:E24">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:36:51, Uncontrolled copy when printed</oddFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:45:09, Uncontrolled copy when printed</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made result file more readavle and saved the last used dir in a JSON file
</commit_message>
<xml_diff>
--- a/TDMS_CSI_ExcelTemplates/Result_Collection_Template.xlsx
+++ b/TDMS_CSI_ExcelTemplates/Result_Collection_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ENTWICKLUNG\Software\data_automator\TDMS_CSI_ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E1011B-B47B-4FFB-82EE-2FD79095D629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60E0AC1-4597-4B4E-88DA-CC836D8DEE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2856" windowWidth="14832" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -374,7 +374,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:45:09, Uncontrolled copy when printed</oddFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-07T14:15:59, Uncontrolled copy when printed</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -383,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B062105E-B73B-455B-ACB6-ED25B9971D91}">
   <dimension ref="B5:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,11 +410,11 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>MAX(Result!D6:AG6)</f>
+        <f>MAX(Result!D6:BZ6)</f>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>MIN(Result!D6:AG6)</f>
+        <f>MIN(Result!D6:BZ6)</f>
         <v>0</v>
       </c>
       <c r="E6">
@@ -428,11 +428,11 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>MAX(Result!D7:AG7)</f>
+        <f>MAX(Result!D7:BZ7)</f>
         <v>0</v>
       </c>
       <c r="D7">
-        <f>MIN(Result!D7:AG7)</f>
+        <f>MIN(Result!D7:BZ7)</f>
         <v>0</v>
       </c>
       <c r="E7">
@@ -446,11 +446,11 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>MAX(Result!D8:AG8)</f>
+        <f>MAX(Result!D8:BZ8)</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>MIN(Result!D8:AG8)</f>
+        <f>MIN(Result!D8:BZ8)</f>
         <v>0</v>
       </c>
       <c r="E8">
@@ -464,11 +464,11 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>MAX(Result!D9:AG9)</f>
+        <f>MAX(Result!D9:BZ9)</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>MIN(Result!D9:AG9)</f>
+        <f>MIN(Result!D9:BZ9)</f>
         <v>0</v>
       </c>
       <c r="E9">
@@ -482,11 +482,11 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>MAX(Result!D10:AG10)</f>
+        <f>MAX(Result!D10:BZ10)</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>MIN(Result!D10:AG10)</f>
+        <f>MIN(Result!D10:BZ10)</f>
         <v>0</v>
       </c>
       <c r="E10">
@@ -500,11 +500,11 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>MAX(Result!D11:AG11)</f>
+        <f>MAX(Result!D11:BZ11)</f>
         <v>0</v>
       </c>
       <c r="D11">
-        <f>MIN(Result!D11:AG11)</f>
+        <f>MIN(Result!D11:BZ11)</f>
         <v>0</v>
       </c>
       <c r="E11">
@@ -518,11 +518,11 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>MAX(Result!D12:AG12)</f>
+        <f>MAX(Result!D12:BZ12)</f>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>MIN(Result!D12:AG12)</f>
+        <f>MIN(Result!D12:BZ12)</f>
         <v>0</v>
       </c>
       <c r="E12">
@@ -536,11 +536,11 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>MAX(Result!D13:AG13)</f>
+        <f>MAX(Result!D13:BZ13)</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>MIN(Result!D13:AG13)</f>
+        <f>MIN(Result!D13:BZ13)</f>
         <v>0</v>
       </c>
       <c r="E13">
@@ -554,11 +554,11 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>MAX(Result!D14:AG14)</f>
+        <f>MAX(Result!D14:BZ14)</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f>MIN(Result!D14:AG14)</f>
+        <f>MIN(Result!D14:BZ14)</f>
         <v>0</v>
       </c>
       <c r="E14">
@@ -572,11 +572,11 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>MAX(Result!D15:AG15)</f>
+        <f>MAX(Result!D15:BZ15)</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>MIN(Result!D15:AG15)</f>
+        <f>MIN(Result!D15:BZ15)</f>
         <v>0</v>
       </c>
       <c r="E15">
@@ -590,11 +590,11 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>MAX(Result!D16:AG16)</f>
+        <f>MAX(Result!D16:BZ16)</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f>MIN(Result!D16:AG16)</f>
+        <f>MIN(Result!D16:BZ16)</f>
         <v>0</v>
       </c>
       <c r="E16">
@@ -608,11 +608,11 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>MAX(Result!D17:AG17)</f>
+        <f>MAX(Result!D17:BZ17)</f>
         <v>0</v>
       </c>
       <c r="D17">
-        <f>MIN(Result!D17:AG17)</f>
+        <f>MIN(Result!D17:BZ17)</f>
         <v>0</v>
       </c>
       <c r="E17">
@@ -626,11 +626,11 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>MAX(Result!D18:AG18)</f>
+        <f>MAX(Result!D18:BZ18)</f>
         <v>0</v>
       </c>
       <c r="D18">
-        <f>MIN(Result!D18:AG18)</f>
+        <f>MIN(Result!D18:BZ18)</f>
         <v>0</v>
       </c>
       <c r="E18">
@@ -644,11 +644,11 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>MAX(Result!D19:AG19)</f>
+        <f>MAX(Result!D19:BZ19)</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f>MIN(Result!D19:AG19)</f>
+        <f>MIN(Result!D19:BZ19)</f>
         <v>0</v>
       </c>
       <c r="E19">
@@ -662,11 +662,11 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>MAX(Result!D20:AG20)</f>
+        <f>MAX(Result!D20:BZ20)</f>
         <v>0</v>
       </c>
       <c r="D20">
-        <f>MIN(Result!D20:AG20)</f>
+        <f>MIN(Result!D20:BZ20)</f>
         <v>0</v>
       </c>
       <c r="E20">
@@ -680,11 +680,11 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>MAX(Result!D21:AG21)</f>
+        <f>MAX(Result!D21:BZ21)</f>
         <v>0</v>
       </c>
       <c r="D21">
-        <f>MIN(Result!D21:AG21)</f>
+        <f>MIN(Result!D21:BZ21)</f>
         <v>0</v>
       </c>
       <c r="E21">
@@ -698,11 +698,11 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>MAX(Result!D22:AG22)</f>
+        <f>MAX(Result!D22:BZ22)</f>
         <v>0</v>
       </c>
       <c r="D22">
-        <f>MIN(Result!D22:AG22)</f>
+        <f>MIN(Result!D22:BZ22)</f>
         <v>0</v>
       </c>
       <c r="E22">
@@ -716,11 +716,11 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>MAX(Result!D23:AG23)</f>
+        <f>MAX(Result!D23:BZ23)</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f>MIN(Result!D23:AG23)</f>
+        <f>MIN(Result!D23:BZ23)</f>
         <v>0</v>
       </c>
       <c r="E23">
@@ -734,11 +734,11 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>MAX(Result!D24:AG24)</f>
+        <f>MAX(Result!D24:BZ24)</f>
         <v>0</v>
       </c>
       <c r="D24">
-        <f>MIN(Result!D24:AG24)</f>
+        <f>MIN(Result!D24:BZ24)</f>
         <v>0</v>
       </c>
       <c r="E24">
@@ -762,7 +762,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-06T22:45:09, Uncontrolled copy when printed</oddFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Akkurat"&amp;7&amp;K737373Classification: Confidential Internal, Creator: thomas.haberkorn@ventrex.com, Date of Classification: 2023-03-07T14:15:59, Uncontrolled copy when printed</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>